<commit_message>
16 Oct update (minor)
</commit_message>
<xml_diff>
--- a/Sources/Commons List.xlsx
+++ b/Sources/Commons List.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SOHABANE\Documents\Projects\Personals\Personal-Hosts\Sources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Programs\Personal-Hosts\Sources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{521F0D2E-D4F5-4845-9505-0345C534F0AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A482508-38CC-45FC-910C-8378A722E76D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{AC752DA5-279B-4E7D-9469-CEF11FD242ED}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{AC752DA5-279B-4E7D-9469-CEF11FD242ED}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -23,9 +23,7 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
     </ext>
@@ -34,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="507" uniqueCount="199">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="513" uniqueCount="201">
   <si>
     <t>0.0.0.0</t>
   </si>
@@ -631,6 +629,12 @@
   </si>
   <si>
     <t>No WWW Required</t>
+  </si>
+  <si>
+    <t>inflact.com</t>
+  </si>
+  <si>
+    <t>simpliers.com</t>
   </si>
 </sst>
 </file>
@@ -699,17 +703,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1024,38 +1027,38 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ECE8835C-5E4A-4A67-BE0B-662B45AD2111}">
-  <dimension ref="A1:J120"/>
+  <dimension ref="A1:J114"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F105" sqref="F105"/>
+      <selection activeCell="C113" sqref="C113:D114"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="26.88671875" customWidth="1"/>
-    <col min="3" max="3" width="9.109375" customWidth="1"/>
-    <col min="4" max="4" width="34.109375" customWidth="1"/>
-    <col min="7" max="7" width="27.33203125" customWidth="1"/>
-    <col min="10" max="10" width="27.33203125" customWidth="1"/>
+    <col min="2" max="2" width="26.85546875" customWidth="1"/>
+    <col min="3" max="3" width="9.140625" customWidth="1"/>
+    <col min="4" max="4" width="34.140625" customWidth="1"/>
+    <col min="7" max="7" width="27.28515625" customWidth="1"/>
+    <col min="10" max="10" width="27.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
         <v>179</v>
       </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="F1" s="3" t="s">
+      <c r="B1" s="3"/>
+      <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
+      <c r="F1" s="4" t="s">
         <v>180</v>
       </c>
-      <c r="G1" s="3"/>
-      <c r="I1" s="3" t="s">
+      <c r="G1" s="4"/>
+      <c r="I1" s="4" t="s">
         <v>198</v>
       </c>
-      <c r="J1" s="3"/>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="J1" s="4"/>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -1082,7 +1085,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>0</v>
       </c>
@@ -1109,7 +1112,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>0</v>
       </c>
@@ -1136,7 +1139,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>0</v>
       </c>
@@ -1159,11 +1162,11 @@
       <c r="I6" t="s">
         <v>0</v>
       </c>
-      <c r="J6" s="5" t="s">
+      <c r="J6" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>0</v>
       </c>
@@ -1186,11 +1189,11 @@
       <c r="I7" t="s">
         <v>0</v>
       </c>
-      <c r="J7" s="5" t="s">
+      <c r="J7" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>0</v>
       </c>
@@ -1213,11 +1216,11 @@
       <c r="I8" t="s">
         <v>0</v>
       </c>
-      <c r="J8" s="5" t="s">
+      <c r="J8" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>0</v>
       </c>
@@ -1240,11 +1243,11 @@
       <c r="I9" t="s">
         <v>0</v>
       </c>
-      <c r="J9" s="5" t="s">
+      <c r="J9" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>0</v>
       </c>
@@ -1267,11 +1270,11 @@
       <c r="I10" t="s">
         <v>0</v>
       </c>
-      <c r="J10" s="5" t="s">
+      <c r="J10" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>0</v>
       </c>
@@ -1292,7 +1295,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>0</v>
       </c>
@@ -1313,7 +1316,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>0</v>
       </c>
@@ -1334,7 +1337,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>0</v>
       </c>
@@ -1355,7 +1358,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>0</v>
       </c>
@@ -1376,7 +1379,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>0</v>
       </c>
@@ -1397,7 +1400,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>0</v>
       </c>
@@ -1418,7 +1421,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>0</v>
       </c>
@@ -1439,7 +1442,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>0</v>
       </c>
@@ -1460,7 +1463,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>0</v>
       </c>
@@ -1481,7 +1484,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>0</v>
       </c>
@@ -1502,7 +1505,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>0</v>
       </c>
@@ -1523,7 +1526,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>0</v>
       </c>
@@ -1544,7 +1547,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>0</v>
       </c>
@@ -1565,7 +1568,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>0</v>
       </c>
@@ -1586,7 +1589,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>0</v>
       </c>
@@ -1607,7 +1610,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>0</v>
       </c>
@@ -1628,7 +1631,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>0</v>
       </c>
@@ -1649,7 +1652,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>0</v>
       </c>
@@ -1670,7 +1673,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>0</v>
       </c>
@@ -1691,7 +1694,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>0</v>
       </c>
@@ -1712,7 +1715,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>0</v>
       </c>
@@ -1733,7 +1736,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>0</v>
       </c>
@@ -1754,7 +1757,7 @@
         <v>177</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>0</v>
       </c>
@@ -1775,7 +1778,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>0</v>
       </c>
@@ -1796,7 +1799,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>0</v>
       </c>
@@ -1817,7 +1820,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>0</v>
       </c>
@@ -1838,7 +1841,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>0</v>
       </c>
@@ -1859,7 +1862,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>0</v>
       </c>
@@ -1880,7 +1883,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>0</v>
       </c>
@@ -1901,7 +1904,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>0</v>
       </c>
@@ -1922,7 +1925,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>0</v>
       </c>
@@ -1943,7 +1946,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>0</v>
       </c>
@@ -1964,7 +1967,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>0</v>
       </c>
@@ -1985,7 +1988,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>0</v>
       </c>
@@ -2006,7 +2009,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>0</v>
       </c>
@@ -2027,7 +2030,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>0</v>
       </c>
@@ -2048,7 +2051,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>0</v>
       </c>
@@ -2069,7 +2072,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>0</v>
       </c>
@@ -2090,7 +2093,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>0</v>
       </c>
@@ -2111,7 +2114,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>0</v>
       </c>
@@ -2132,7 +2135,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>0</v>
       </c>
@@ -2153,7 +2156,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>0</v>
       </c>
@@ -2174,7 +2177,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>0</v>
       </c>
@@ -2195,7 +2198,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>0</v>
       </c>
@@ -2216,7 +2219,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>0</v>
       </c>
@@ -2237,7 +2240,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>0</v>
       </c>
@@ -2258,7 +2261,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>0</v>
       </c>
@@ -2279,7 +2282,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>0</v>
       </c>
@@ -2300,7 +2303,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>0</v>
       </c>
@@ -2321,7 +2324,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>0</v>
       </c>
@@ -2342,7 +2345,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>0</v>
       </c>
@@ -2363,7 +2366,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>0</v>
       </c>
@@ -2384,7 +2387,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>0</v>
       </c>
@@ -2405,7 +2408,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>0</v>
       </c>
@@ -2426,7 +2429,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="66" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>0</v>
       </c>
@@ -2447,7 +2450,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="67" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>0</v>
       </c>
@@ -2468,7 +2471,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="68" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>0</v>
       </c>
@@ -2479,7 +2482,7 @@
         <v>0</v>
       </c>
       <c r="D68" t="str">
-        <f t="shared" ref="D68:D112" si="1">_xlfn.CONCAT("www.",B68)</f>
+        <f t="shared" ref="D68:D114" si="1">_xlfn.CONCAT("www.",B68)</f>
         <v>www.mythreadreader.com</v>
       </c>
       <c r="F68" s="1" t="s">
@@ -2489,7 +2492,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="69" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>0</v>
       </c>
@@ -2510,7 +2513,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="70" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>0</v>
       </c>
@@ -2531,7 +2534,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="71" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>0</v>
       </c>
@@ -2552,7 +2555,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="72" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>0</v>
       </c>
@@ -2573,7 +2576,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="73" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>0</v>
       </c>
@@ -2594,7 +2597,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="74" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>0</v>
       </c>
@@ -2615,7 +2618,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="75" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>0</v>
       </c>
@@ -2636,7 +2639,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="76" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>0</v>
       </c>
@@ -2657,7 +2660,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="77" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>0</v>
       </c>
@@ -2678,7 +2681,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="78" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>0</v>
       </c>
@@ -2699,7 +2702,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="79" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>0</v>
       </c>
@@ -2720,7 +2723,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="80" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>0</v>
       </c>
@@ -2741,11 +2744,11 @@
         <v>170</v>
       </c>
     </row>
-    <row r="81" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>0</v>
       </c>
-      <c r="B81" s="4" t="s">
+      <c r="B81" s="2" t="s">
         <v>186</v>
       </c>
       <c r="C81" t="s">
@@ -2762,7 +2765,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="82" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>0</v>
       </c>
@@ -2777,7 +2780,7 @@
         <v>www.save-insta.com</v>
       </c>
     </row>
-    <row r="83" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>0</v>
       </c>
@@ -2792,7 +2795,7 @@
         <v>www.smihub.com</v>
       </c>
     </row>
-    <row r="84" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>0</v>
       </c>
@@ -2807,7 +2810,7 @@
         <v>www.sotwe.com</v>
       </c>
     </row>
-    <row r="85" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>0</v>
       </c>
@@ -2822,7 +2825,7 @@
         <v>www.storiesdown.com</v>
       </c>
     </row>
-    <row r="86" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>0</v>
       </c>
@@ -2837,7 +2840,7 @@
         <v>www.storiesig.app</v>
       </c>
     </row>
-    <row r="87" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>0</v>
       </c>
@@ -2852,7 +2855,7 @@
         <v>www.storiesig.info</v>
       </c>
     </row>
-    <row r="88" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>0</v>
       </c>
@@ -2867,7 +2870,7 @@
         <v>www.storiesig.me</v>
       </c>
     </row>
-    <row r="89" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>0</v>
       </c>
@@ -2882,7 +2885,7 @@
         <v>www.storiesig.net</v>
       </c>
     </row>
-    <row r="90" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>0</v>
       </c>
@@ -2897,7 +2900,7 @@
         <v>www.storieswatch.com</v>
       </c>
     </row>
-    <row r="91" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>0</v>
       </c>
@@ -2912,7 +2915,7 @@
         <v>www.storysaver.net</v>
       </c>
     </row>
-    <row r="92" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>0</v>
       </c>
@@ -2927,14 +2930,14 @@
         <v>www.stweetly.com</v>
       </c>
     </row>
-    <row r="93" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A93" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="B93" s="5" t="s">
+    <row r="93" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A93" t="s">
+        <v>0</v>
+      </c>
+      <c r="B93" t="s">
         <v>126</v>
       </c>
-      <c r="C93" s="5" t="s">
+      <c r="C93" t="s">
         <v>0</v>
       </c>
       <c r="D93" t="str">
@@ -2942,7 +2945,7 @@
         <v>www.t.com.sb</v>
       </c>
     </row>
-    <row r="94" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>0</v>
       </c>
@@ -2957,7 +2960,7 @@
         <v>www.thepicgram.com</v>
       </c>
     </row>
-    <row r="95" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>0</v>
       </c>
@@ -2972,7 +2975,7 @@
         <v>www.threadreaderapp.com</v>
       </c>
     </row>
-    <row r="96" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>0</v>
       </c>
@@ -2987,7 +2990,7 @@
         <v>www.tweepsmap.com</v>
       </c>
     </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>0</v>
       </c>
@@ -3002,7 +3005,7 @@
         <v>www.tweepy.net</v>
       </c>
     </row>
-    <row r="98" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>0</v>
       </c>
@@ -3017,7 +3020,7 @@
         <v>www.tweetbeam.com</v>
       </c>
     </row>
-    <row r="99" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>0</v>
       </c>
@@ -3032,7 +3035,7 @@
         <v>www.twidoom.com</v>
       </c>
     </row>
-    <row r="100" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>0</v>
       </c>
@@ -3047,7 +3050,7 @@
         <v>www.twiiit.com</v>
       </c>
     </row>
-    <row r="101" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>0</v>
       </c>
@@ -3062,7 +3065,7 @@
         <v>www.twimfeed.com</v>
       </c>
     </row>
-    <row r="102" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>0</v>
       </c>
@@ -3077,7 +3080,7 @@
         <v>www.twimg.com</v>
       </c>
     </row>
-    <row r="103" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>0</v>
       </c>
@@ -3092,7 +3095,7 @@
         <v>www.twipho.net</v>
       </c>
     </row>
-    <row r="104" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>0</v>
       </c>
@@ -3107,7 +3110,7 @@
         <v>www.twipu.net</v>
       </c>
     </row>
-    <row r="105" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
         <v>0</v>
       </c>
@@ -3122,7 +3125,7 @@
         <v>www.twitter.com</v>
       </c>
     </row>
-    <row r="106" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
         <v>0</v>
       </c>
@@ -3137,7 +3140,7 @@
         <v>www.twittertt.com</v>
       </c>
     </row>
-    <row r="107" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
         <v>0</v>
       </c>
@@ -3152,7 +3155,7 @@
         <v>www.twubs.com</v>
       </c>
     </row>
-    <row r="108" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
         <v>0</v>
       </c>
@@ -3167,7 +3170,7 @@
         <v>www.viewerig.com</v>
       </c>
     </row>
-    <row r="109" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
         <v>0</v>
       </c>
@@ -3182,7 +3185,7 @@
         <v>www.viewprivateinsta.com</v>
       </c>
     </row>
-    <row r="110" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
         <v>0</v>
       </c>
@@ -3197,7 +3200,7 @@
         <v>www.visibletweets.com</v>
       </c>
     </row>
-    <row r="111" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
         <v>0</v>
       </c>
@@ -3212,7 +3215,7 @@
         <v>www.watchinsta.com</v>
       </c>
     </row>
-    <row r="112" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
         <v>0</v>
       </c>
@@ -3227,17 +3230,35 @@
         <v>www.webstagram.org</v>
       </c>
     </row>
-    <row r="118" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A118" s="5"/>
-      <c r="B118" s="5"/>
-      <c r="C118" s="5"/>
-      <c r="D118" s="5"/>
-    </row>
-    <row r="120" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A120" s="5"/>
-      <c r="B120" s="5"/>
-      <c r="C120" s="5"/>
-      <c r="D120" s="5"/>
+    <row r="113" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A113" t="s">
+        <v>0</v>
+      </c>
+      <c r="B113" t="s">
+        <v>199</v>
+      </c>
+      <c r="C113" t="s">
+        <v>0</v>
+      </c>
+      <c r="D113" t="str">
+        <f t="shared" si="1"/>
+        <v>www.inflact.com</v>
+      </c>
+    </row>
+    <row r="114" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A114" t="s">
+        <v>0</v>
+      </c>
+      <c r="B114" t="s">
+        <v>200</v>
+      </c>
+      <c r="C114" t="s">
+        <v>0</v>
+      </c>
+      <c r="D114" t="str">
+        <f t="shared" si="1"/>
+        <v>www.simpliers.com</v>
+      </c>
     </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="D3:D117">

</xml_diff>